<commit_message>
Removed AZ naming Adjustment to Trade matrix making the trades working more clearly and split into bi and uni trade links
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -5,18 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\Trades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\DTU\TIMES-DE\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDE2B4-EB3A-4A64-B350-9F458E24A799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002E40CD-2C02-4B2A-9666-004A2D073C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14136" yWindow="348" windowWidth="25704" windowHeight="15948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ELCC" sheetId="5" r:id="rId1"/>
-    <sheet name="35 (2)" sheetId="6" r:id="rId2"/>
-    <sheet name="HETC" sheetId="10" r:id="rId3"/>
-    <sheet name="HETD" sheetId="11" r:id="rId4"/>
+    <sheet name="BI" sheetId="13" r:id="rId1"/>
+    <sheet name="Uni" sheetId="5" r:id="rId2"/>
+    <sheet name="35 (2)" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="248">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -860,7 +859,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -975,6 +974,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -988,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1054,6 +1059,8 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,7 +1079,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1391,25 +1398,280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F781D5-E7FF-452F-B049-9C2EDF8539B3}">
+  <dimension ref="B3:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K14:K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="31"/>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="30">
+        <v>1</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="27">
+        <v>1</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="27">
+        <v>1</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="27">
+        <v>1</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C3:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1435,11 +1697,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="26"/>
       <c r="K5" t="s">
         <v>8</v>
@@ -1448,20 +1710,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="K6" t="s">
         <v>9</v>
       </c>
@@ -1469,22 +1725,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
+      <c r="F7" s="32"/>
       <c r="K7" t="s">
         <v>10</v>
       </c>
@@ -1492,38 +1740,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
         <v>11</v>
       </c>
@@ -1534,27 +1769,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet49">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:AV177"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="4" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" style="4"/>
+    <col min="2" max="2" width="3.77734375" style="4"/>
     <col min="3" max="24" width="6" style="4" customWidth="1"/>
-    <col min="25" max="33" width="5.36328125" style="4" customWidth="1"/>
-    <col min="34" max="16384" width="3.81640625" style="4"/>
+    <col min="25" max="33" width="5.33203125" style="4" customWidth="1"/>
+    <col min="34" max="16384" width="3.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>245</v>
       </c>
@@ -1601,7 +1836,7 @@
       <c r="AU1"/>
       <c r="AV1"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>244</v>
       </c>
@@ -1648,7 +1883,7 @@
       <c r="AU2"/>
       <c r="AV2"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>243</v>
       </c>
@@ -1695,7 +1930,7 @@
       <c r="AU3"/>
       <c r="AV3"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1739,7 +1974,7 @@
       <c r="AU4"/>
       <c r="AV4"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>242</v>
       </c>
@@ -1786,7 +2021,7 @@
       <c r="AU5"/>
       <c r="AV5"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>241</v>
       </c>
@@ -1833,7 +2068,7 @@
       <c r="AU6"/>
       <c r="AV6"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>240</v>
       </c>
@@ -1880,7 +2115,7 @@
       <c r="AU7"/>
       <c r="AV7"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>239</v>
       </c>
@@ -1927,7 +2162,7 @@
       <c r="AU8"/>
       <c r="AV8"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>238</v>
       </c>
@@ -1974,7 +2209,7 @@
       <c r="AU9"/>
       <c r="AV9"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>237</v>
       </c>
@@ -2021,7 +2256,7 @@
       <c r="AU10"/>
       <c r="AV10"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>236</v>
       </c>
@@ -2068,7 +2303,7 @@
       <c r="AU11"/>
       <c r="AV11"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>235</v>
       </c>
@@ -2118,7 +2353,7 @@
       <c r="AU12"/>
       <c r="AV12"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>234</v>
       </c>
@@ -2168,7 +2403,7 @@
       <c r="AU13"/>
       <c r="AV13"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>233</v>
       </c>
@@ -2218,7 +2453,7 @@
       <c r="AU14"/>
       <c r="AV14"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2266,7 +2501,7 @@
       <c r="AU15"/>
       <c r="AV15"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2310,7 +2545,7 @@
       <c r="AU16"/>
       <c r="AV16"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>232</v>
       </c>
@@ -2362,7 +2597,7 @@
       <c r="AU17"/>
       <c r="AV17"/>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
@@ -2471,7 +2706,7 @@
       <c r="AU18"/>
       <c r="AV18"/>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2016</v>
       </c>
@@ -2525,7 +2760,7 @@
       <c r="AU19"/>
       <c r="AV19"/>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2016</v>
       </c>
@@ -2589,7 +2824,7 @@
       <c r="AU20"/>
       <c r="AV20"/>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>2016</v>
       </c>
@@ -2653,7 +2888,7 @@
       <c r="AU21"/>
       <c r="AV21"/>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2016</v>
       </c>
@@ -2721,7 +2956,7 @@
       <c r="AU22"/>
       <c r="AV22"/>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2016</v>
       </c>
@@ -2789,7 +3024,7 @@
       <c r="AU23"/>
       <c r="AV23"/>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2016</v>
       </c>
@@ -2853,7 +3088,7 @@
       <c r="AU24"/>
       <c r="AV24"/>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>2016</v>
       </c>
@@ -2915,7 +3150,7 @@
       <c r="AU25"/>
       <c r="AV25"/>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>2016</v>
       </c>
@@ -2969,7 +3204,7 @@
       <c r="AU26"/>
       <c r="AV26"/>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>2016</v>
       </c>
@@ -3024,7 +3259,7 @@
       <c r="AU27"/>
       <c r="AV27"/>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>2016</v>
       </c>
@@ -3086,7 +3321,7 @@
       <c r="AU28"/>
       <c r="AV28"/>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>2016</v>
       </c>
@@ -3140,7 +3375,7 @@
       <c r="AU29"/>
       <c r="AV29"/>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>2016</v>
       </c>
@@ -3196,7 +3431,7 @@
       <c r="AU30"/>
       <c r="AV30"/>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>2016</v>
       </c>
@@ -3250,7 +3485,7 @@
       <c r="AU31"/>
       <c r="AV31"/>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>2016</v>
       </c>
@@ -3308,7 +3543,7 @@
       <c r="AU32"/>
       <c r="AV32"/>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>2016</v>
       </c>
@@ -3372,7 +3607,7 @@
       <c r="AU33"/>
       <c r="AV33"/>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>2016</v>
       </c>
@@ -3436,7 +3671,7 @@
       <c r="AU34"/>
       <c r="AV34"/>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>2016</v>
       </c>
@@ -3500,7 +3735,7 @@
       <c r="AU35"/>
       <c r="AV35"/>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>2016</v>
       </c>
@@ -3562,7 +3797,7 @@
       <c r="AU36"/>
       <c r="AV36"/>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>2016</v>
       </c>
@@ -3624,7 +3859,7 @@
       <c r="AU37"/>
       <c r="AV37"/>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>2016</v>
       </c>
@@ -3681,7 +3916,7 @@
       <c r="AU38"/>
       <c r="AV38"/>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>2016</v>
       </c>
@@ -3743,7 +3978,7 @@
       <c r="AU39"/>
       <c r="AV39"/>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>2016</v>
       </c>
@@ -3807,7 +4042,7 @@
       <c r="AU40"/>
       <c r="AV40"/>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>2016</v>
       </c>
@@ -3873,7 +4108,7 @@
       <c r="AU41"/>
       <c r="AV41"/>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>2016</v>
       </c>
@@ -3939,7 +4174,7 @@
       <c r="AU42"/>
       <c r="AV42"/>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>2016</v>
       </c>
@@ -4001,7 +4236,7 @@
       <c r="AU43"/>
       <c r="AV43"/>
     </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>2016</v>
       </c>
@@ -4065,7 +4300,7 @@
       <c r="AU44"/>
       <c r="AV44"/>
     </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>2016</v>
       </c>
@@ -4129,7 +4364,7 @@
       <c r="AU45"/>
       <c r="AV45"/>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>2016</v>
       </c>
@@ -4193,7 +4428,7 @@
       <c r="AU46"/>
       <c r="AV46"/>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>2016</v>
       </c>
@@ -4253,7 +4488,7 @@
       <c r="AU47"/>
       <c r="AV47"/>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>2016</v>
       </c>
@@ -4311,7 +4546,7 @@
       <c r="AU48"/>
       <c r="AV48"/>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>200</v>
       </c>
@@ -4348,7 +4583,7 @@
       <c r="AU49"/>
       <c r="AV49"/>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>199</v>
       </c>
@@ -4385,7 +4620,7 @@
       <c r="AU50"/>
       <c r="AV50"/>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="L51" s="12"/>
@@ -4419,7 +4654,7 @@
       <c r="AU51"/>
       <c r="AV51"/>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="L52" s="12"/>
@@ -4453,7 +4688,7 @@
       <c r="AU52"/>
       <c r="AV52"/>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="L53" s="12"/>
@@ -4487,7 +4722,7 @@
       <c r="AU53"/>
       <c r="AV53"/>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="L54" s="12"/>
@@ -4521,7 +4756,7 @@
       <c r="AU54"/>
       <c r="AV54"/>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>198</v>
       </c>
@@ -4557,7 +4792,7 @@
       <c r="AU55"/>
       <c r="AV55"/>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>197</v>
       </c>
@@ -4597,7 +4832,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>195</v>
       </c>
@@ -4637,7 +4872,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>193</v>
       </c>
@@ -4677,7 +4912,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>191</v>
       </c>
@@ -4717,7 +4952,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>189</v>
       </c>
@@ -4757,7 +4992,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>187</v>
       </c>
@@ -4797,7 +5032,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>185</v>
       </c>
@@ -4837,7 +5072,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>183</v>
       </c>
@@ -4877,7 +5112,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>181</v>
       </c>
@@ -4917,7 +5152,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>179</v>
       </c>
@@ -4957,7 +5192,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>177</v>
       </c>
@@ -4997,7 +5232,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>175</v>
       </c>
@@ -5037,7 +5272,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>173</v>
       </c>
@@ -5077,7 +5312,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>171</v>
       </c>
@@ -5117,7 +5352,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>169</v>
       </c>
@@ -5157,7 +5392,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>168</v>
       </c>
@@ -5197,7 +5432,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>167</v>
       </c>
@@ -5237,7 +5472,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>166</v>
       </c>
@@ -5277,7 +5512,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>164</v>
       </c>
@@ -5317,7 +5552,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>162</v>
       </c>
@@ -5357,7 +5592,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>161</v>
       </c>
@@ -5397,7 +5632,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>160</v>
       </c>
@@ -5437,7 +5672,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>159</v>
       </c>
@@ -5477,7 +5712,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>157</v>
       </c>
@@ -5517,7 +5752,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
         <v>156</v>
       </c>
@@ -5557,7 +5792,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
         <v>155</v>
       </c>
@@ -5597,7 +5832,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
         <v>153</v>
       </c>
@@ -5637,7 +5872,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -5672,7 +5907,7 @@
       <c r="AF83"/>
       <c r="AG83"/>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A84" s="11"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -5707,7 +5942,7 @@
       <c r="AF84"/>
       <c r="AG84"/>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>151</v>
       </c>
@@ -5744,7 +5979,7 @@
       <c r="AF85"/>
       <c r="AG85"/>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>150</v>
       </c>
@@ -5784,7 +6019,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>148</v>
       </c>
@@ -5824,7 +6059,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A88" s="11" t="s">
         <v>146</v>
       </c>
@@ -5864,7 +6099,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
         <v>143</v>
       </c>
@@ -5904,7 +6139,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
         <v>143</v>
       </c>
@@ -5944,7 +6179,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
         <v>142</v>
       </c>
@@ -5984,7 +6219,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
         <v>140</v>
       </c>
@@ -6024,7 +6259,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93" s="11" t="s">
         <v>138</v>
       </c>
@@ -6064,7 +6299,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A94" s="11" t="s">
         <v>136</v>
       </c>
@@ -6104,7 +6339,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A95" s="11" t="s">
         <v>134</v>
       </c>
@@ -6144,7 +6379,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
         <v>133</v>
       </c>
@@ -6184,7 +6419,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A97" s="11" t="s">
         <v>132</v>
       </c>
@@ -6224,7 +6459,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A98" s="11" t="s">
         <v>131</v>
       </c>
@@ -6264,7 +6499,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A99" s="11" t="s">
         <v>130</v>
       </c>
@@ -6304,7 +6539,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A100" s="11" t="s">
         <v>128</v>
       </c>
@@ -6344,7 +6579,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A101" s="11" t="s">
         <v>126</v>
       </c>
@@ -6384,7 +6619,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A102" s="11" t="s">
         <v>124</v>
       </c>
@@ -6424,7 +6659,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A103" s="11" t="s">
         <v>122</v>
       </c>
@@ -6464,7 +6699,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
         <v>120</v>
       </c>
@@ -6504,7 +6739,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A105" s="11" t="s">
         <v>118</v>
       </c>
@@ -6544,7 +6779,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A106" s="11" t="s">
         <v>116</v>
       </c>
@@ -6584,7 +6819,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A107" s="11" t="s">
         <v>114</v>
       </c>
@@ -6624,7 +6859,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A108" s="11" t="s">
         <v>112</v>
       </c>
@@ -6664,7 +6899,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A109" s="11" t="s">
         <v>110</v>
       </c>
@@ -6704,7 +6939,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A110" s="11" t="s">
         <v>108</v>
       </c>
@@ -6744,7 +6979,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A111" s="11" t="s">
         <v>106</v>
       </c>
@@ -6784,7 +7019,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A112" s="11" t="s">
         <v>104</v>
       </c>
@@ -6824,7 +7059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A113" s="11" t="s">
         <v>100</v>
       </c>
@@ -6864,7 +7099,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A114" s="11" t="s">
         <v>98</v>
       </c>
@@ -6904,7 +7139,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>100</v>
       </c>
@@ -6944,7 +7179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>98</v>
       </c>
@@ -6984,7 +7219,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
         <v>96</v>
       </c>
@@ -7024,7 +7259,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A118" s="11" t="s">
         <v>94</v>
       </c>
@@ -7064,7 +7299,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A119" s="11" t="s">
         <v>92</v>
       </c>
@@ -7104,7 +7339,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A120" s="11" t="s">
         <v>90</v>
       </c>
@@ -7144,7 +7379,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A121" s="11" t="s">
         <v>88</v>
       </c>
@@ -7184,7 +7419,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A122" s="11" t="s">
         <v>86</v>
       </c>
@@ -7224,7 +7459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A123" s="11" t="s">
         <v>84</v>
       </c>
@@ -7264,7 +7499,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A124" s="11" t="s">
         <v>82</v>
       </c>
@@ -7304,7 +7539,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
         <v>80</v>
       </c>
@@ -7344,7 +7579,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>78</v>
       </c>
@@ -7384,7 +7619,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A127" s="11" t="s">
         <v>76</v>
       </c>
@@ -7424,7 +7659,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
         <v>75</v>
       </c>
@@ -7464,7 +7699,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A129" s="11"/>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
@@ -7499,7 +7734,7 @@
       <c r="AF129"/>
       <c r="AG129"/>
     </row>
-    <row r="130" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A130" s="11" t="s">
         <v>73</v>
       </c>
@@ -7542,7 +7777,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A131" s="11" t="s">
         <v>70</v>
       </c>
@@ -7581,7 +7816,7 @@
       <c r="AU131"/>
       <c r="AV131"/>
     </row>
-    <row r="132" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A132" s="11" t="s">
         <v>69</v>
       </c>
@@ -7627,7 +7862,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="133" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A133" s="11" t="s">
         <v>67</v>
       </c>
@@ -7670,7 +7905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A134" s="11" t="s">
         <v>65</v>
       </c>
@@ -7716,7 +7951,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="135" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A135" s="11" t="s">
         <v>63</v>
       </c>
@@ -7759,7 +7994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A136" s="11" t="s">
         <v>61</v>
       </c>
@@ -7805,7 +8040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A137" s="11" t="s">
         <v>59</v>
       </c>
@@ -7848,7 +8083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A138" s="11" t="s">
         <v>57</v>
       </c>
@@ -7894,7 +8129,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="139" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A139" s="11" t="s">
         <v>55</v>
       </c>
@@ -7937,7 +8172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A140" s="11" t="s">
         <v>53</v>
       </c>
@@ -7983,7 +8218,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="141" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A141" s="11" t="s">
         <v>51</v>
       </c>
@@ -8026,7 +8261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A142" s="11" t="s">
         <v>49</v>
       </c>
@@ -8072,7 +8307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A143" s="11" t="s">
         <v>47</v>
       </c>
@@ -8115,7 +8350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A144" s="11" t="s">
         <v>45</v>
       </c>
@@ -8161,7 +8396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A145" s="11" t="s">
         <v>43</v>
       </c>
@@ -8204,7 +8439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A146" s="11" t="s">
         <v>41</v>
       </c>
@@ -8250,7 +8485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
         <v>39</v>
       </c>
@@ -8293,7 +8528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A148" s="11" t="s">
         <v>37</v>
       </c>
@@ -8339,7 +8574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A149" s="11" t="s">
         <v>35</v>
       </c>
@@ -8382,7 +8617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A150" s="11" t="s">
         <v>33</v>
       </c>
@@ -8428,7 +8663,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="151" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A151" s="11" t="s">
         <v>31</v>
       </c>
@@ -8471,7 +8706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A152" s="11" t="s">
         <v>29</v>
       </c>
@@ -8517,7 +8752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A153" s="11" t="s">
         <v>27</v>
       </c>
@@ -8560,7 +8795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A154" s="11" t="s">
         <v>25</v>
       </c>
@@ -8606,7 +8841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A155" s="11" t="s">
         <v>23</v>
       </c>
@@ -8649,7 +8884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A156" s="11" t="s">
         <v>21</v>
       </c>
@@ -8695,7 +8930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A157" s="11" t="s">
         <v>19</v>
       </c>
@@ -8738,7 +8973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A158" s="11" t="s">
         <v>17</v>
       </c>
@@ -8784,7 +9019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A159" s="11" t="s">
         <v>15</v>
       </c>
@@ -8829,7 +9064,7 @@
       <c r="AU159"/>
       <c r="AV159"/>
     </row>
-    <row r="160" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A160" s="11" t="s">
         <v>12</v>
       </c>
@@ -8866,7 +9101,7 @@
       <c r="AU160"/>
       <c r="AV160"/>
     </row>
-    <row r="162" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
@@ -8879,7 +9114,7 @@
       <c r="J162" s="6"/>
       <c r="K162" s="6"/>
     </row>
-    <row r="163" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="8"/>
@@ -8891,7 +9126,7 @@
       <c r="I163" s="8"/>
       <c r="J163" s="6"/>
     </row>
-    <row r="164" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
@@ -8903,7 +9138,7 @@
       <c r="I164" s="6"/>
       <c r="J164" s="6"/>
     </row>
-    <row r="165" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
@@ -8915,7 +9150,7 @@
       <c r="I165" s="8"/>
       <c r="J165" s="6"/>
     </row>
-    <row r="166" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
@@ -8927,7 +9162,7 @@
       <c r="I166" s="6"/>
       <c r="J166" s="8"/>
     </row>
-    <row r="167" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
@@ -8939,7 +9174,7 @@
       <c r="I167" s="6"/>
       <c r="J167" s="8"/>
     </row>
-    <row r="168" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
@@ -8951,7 +9186,7 @@
       <c r="I168" s="6"/>
       <c r="J168" s="8"/>
     </row>
-    <row r="169" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -8963,7 +9198,7 @@
       <c r="I169" s="6"/>
       <c r="J169" s="8"/>
     </row>
-    <row r="170" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -8975,7 +9210,7 @@
       <c r="I170" s="6"/>
       <c r="J170" s="6"/>
     </row>
-    <row r="171" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
@@ -8987,7 +9222,7 @@
       <c r="I171" s="6"/>
       <c r="J171" s="6"/>
     </row>
-    <row r="172" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
@@ -8999,7 +9234,7 @@
       <c r="I172" s="6"/>
       <c r="J172" s="6"/>
     </row>
-    <row r="173" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
@@ -9011,7 +9246,7 @@
       <c r="I173" s="6"/>
       <c r="J173" s="6"/>
     </row>
-    <row r="174" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -9023,7 +9258,7 @@
       <c r="I174" s="8"/>
       <c r="J174" s="6"/>
     </row>
-    <row r="175" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
@@ -9035,7 +9270,7 @@
       <c r="I175" s="6"/>
       <c r="J175" s="8"/>
     </row>
-    <row r="176" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -9047,7 +9282,7 @@
       <c r="I176" s="8"/>
       <c r="J176" s="6"/>
     </row>
-    <row r="177" spans="1:11" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -9069,239 +9304,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="C3:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="26">
-        <v>1</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="C3:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C4" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C5" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C6" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="30">
-        <v>1</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="27">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="27">
-        <v>1</v>
-      </c>
-      <c r="E7" s="27">
-        <v>1</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27">
-        <v>1</v>
-      </c>
-      <c r="H7" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="27">
-        <v>1</v>
-      </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="27">
-        <v>1</v>
-      </c>
-      <c r="E9" s="27">
-        <v>1</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
-        <v>1</v>
-      </c>
-      <c r="H9" s="27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -9309,6 +9311,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -9531,15 +9542,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B9EB0F-9E18-4488-856E-561DDDE8EE50}">
   <ds:schemaRefs>
@@ -9550,6 +9552,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F21AFFA6-4B3D-491D-AC34-DD4539DE7BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DC82FAE-D590-4BE2-94FA-6638E43DC438}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9566,12 +9576,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F21AFFA6-4B3D-491D-AC34-DD4539DE7BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>